<commit_message>
tax time and some folder restructuring
</commit_message>
<xml_diff>
--- a/2 - Salary/Sal Summary.xlsx
+++ b/2 - Salary/Sal Summary.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/anand_nidamanuru_sap_com/Documents/Sync/Paisa/2 - Salary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{8D1F6C08-F22E-4447-974E-D374FCF62DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FCBBBE36-E77C-3C4A-B211-41B2ACA257E2}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{8D1F6C08-F22E-4447-974E-D374FCF62DB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9DF39D2A-57F2-2D45-AB11-A84A4ECC95A4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" activeTab="1" xr2:uid="{F0DE16E1-F8FD-3548-B840-BF99186538BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" activeTab="1" xr2:uid="{F0DE16E1-F8FD-3548-B840-BF99186538BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="2020-Dec Hike" sheetId="2" r:id="rId2"/>
+    <sheet name="Actuals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Month</t>
   </si>
@@ -113,6 +113,75 @@
   </si>
   <si>
     <t>Actual paid in Mar next year</t>
+  </si>
+  <si>
+    <t>Salary as per hike doc</t>
+  </si>
+  <si>
+    <t>Variable Pay</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Apr-2010 to Mar-2011</t>
+  </si>
+  <si>
+    <t>Apr-2011 to Mar-2012</t>
+  </si>
+  <si>
+    <t>Apr-2012 to Mar-2013</t>
+  </si>
+  <si>
+    <t>Apr-2013 to Sep-2013</t>
+  </si>
+  <si>
+    <t>Oct-2013 to Mar-2014</t>
+  </si>
+  <si>
+    <t>Apr-2014 to Mar-2015</t>
+  </si>
+  <si>
+    <t>Apr-2015 to Mar-2016</t>
+  </si>
+  <si>
+    <t>Apr-2016 to Mar-2017</t>
+  </si>
+  <si>
+    <t>Apr-2017 to Mar-2018</t>
+  </si>
+  <si>
+    <t>Apr-2018 to Mar-2019</t>
+  </si>
+  <si>
+    <t>Apr-2019 to Mar-2020</t>
+  </si>
+  <si>
+    <t>Apr-2020 to Nov-2020</t>
+  </si>
+  <si>
+    <t>Dec-2020 to Mar-2021</t>
+  </si>
+  <si>
+    <t>Hike%</t>
+  </si>
+  <si>
+    <t>Actual Bonus in Sal</t>
+  </si>
+  <si>
+    <t>Mid yr hike</t>
+  </si>
+  <si>
+    <t>Bonus %</t>
+  </si>
+  <si>
+    <t>Bonus payout in March 2021 will be for the last year. That is from 01-Jan-2020 to 31-Dec-2020</t>
+  </si>
+  <si>
+    <t>Bonus of Jan to Mar 2020 with 2019 FY sal + Bonus of Apr 2020 to Dec 2020 with 2020 FY Sal</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -136,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +230,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -174,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -183,7 +258,15 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -504,7 +587,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,10 +602,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1193,10 +1276,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="8"/>
+      <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -1320,12 +1403,426 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FCFE06-4DA0-4D44-918E-D69DB73DA340}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="80.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="H1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1103832.68</v>
+      </c>
+      <c r="B3" s="4">
+        <f>A3-C3</f>
+        <v>976774.67999999993</v>
+      </c>
+      <c r="C3" s="4">
+        <v>127058</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3">
+        <v>170313.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <f>B4+C4</f>
+        <v>1302523.08</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1152385.08</v>
+      </c>
+      <c r="C4" s="4">
+        <v>150138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <f>ROUND((A4-A3)/A3*100,1)</f>
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <f>C3*3/12 + C4*9/12</f>
+        <v>144368</v>
+      </c>
+      <c r="I4">
+        <v>144246.49</v>
+      </c>
+      <c r="J4">
+        <f>ROUND(I4/H4*100,1)</f>
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1613082.08</v>
+      </c>
+      <c r="B5" s="4">
+        <f>A5-C5</f>
+        <v>1374055.08</v>
+      </c>
+      <c r="C5" s="8">
+        <v>239027</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E15" si="0">ROUND((A5-A4)/A4*100,1)</f>
+        <v>23.8</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5" si="1">C4*3/12 + C5*9/12</f>
+        <v>216804.75</v>
+      </c>
+      <c r="I5">
+        <v>190508.91</v>
+      </c>
+      <c r="J5">
+        <f>ROUND(I5/H5*100,1)</f>
+        <v>87.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>1761487.48</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1497264.48</v>
+      </c>
+      <c r="C6" s="11">
+        <v>264223</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="12">
+        <f>C5*3/12 + C6*6/12</f>
+        <v>191868.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <f>B7+C7</f>
+        <v>2204094</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1807356</v>
+      </c>
+      <c r="C7" s="4">
+        <v>396738</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>25.1</v>
+      </c>
+      <c r="H7">
+        <f>H6+C7*3/12</f>
+        <v>291052.75</v>
+      </c>
+      <c r="I7">
+        <v>300000</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J13" si="2">ROUND(I7/H7*100,1)</f>
+        <v>103.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>2243559.7599999998</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1839719.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>403840</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="H8">
+        <v>402088.82</v>
+      </c>
+      <c r="I8">
+        <v>402089</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>2669028.04</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2135225.04</v>
+      </c>
+      <c r="C9" s="4">
+        <v>533803</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H9" s="4">
+        <v>501757.33</v>
+      </c>
+      <c r="I9">
+        <v>605069</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>120.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>3102970.2</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2482378.2000000002</v>
+      </c>
+      <c r="C10" s="4">
+        <v>620592</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>16.3</v>
+      </c>
+      <c r="H10" s="4">
+        <v>599013.31000000006</v>
+      </c>
+      <c r="I10">
+        <v>716839</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>119.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>3601265.48</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2881014.48</v>
+      </c>
+      <c r="C11" s="4">
+        <v>720251</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H11" s="4">
+        <v>695677.54</v>
+      </c>
+      <c r="I11">
+        <v>723505</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>3941488.28</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3221237.28</v>
+      </c>
+      <c r="C12" s="4">
+        <v>720251</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="H12">
+        <v>720251</v>
+      </c>
+      <c r="I12">
+        <v>792276</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>4141488</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3421237</v>
+      </c>
+      <c r="C13" s="4">
+        <v>720251</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H13">
+        <v>720251</v>
+      </c>
+      <c r="I13">
+        <v>849896</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>4493514</v>
+      </c>
+      <c r="B14" s="10">
+        <v>3773263</v>
+      </c>
+      <c r="C14" s="10">
+        <v>720251</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="12">
+        <f>C13*3/12 + C14*8/12</f>
+        <v>660230.08333333326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>5135637</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4312462</v>
+      </c>
+      <c r="C15" s="4">
+        <v>823175</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>14.3</v>
+      </c>
+      <c r="H15">
+        <f>H14+C15*1/12</f>
+        <v>728827.99999999988</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>